<commit_message>
changed type of stmod connector. from .2mm to .4mm
</commit_message>
<xml_diff>
--- a/5_Hardware/PCB_EXTENSION_CircuitVoyager_pre1/Project Outputs for PCB_EXT_CV_PRE1/BOM/BOM-PCB_EXT_CV_PRE1.xlsx
+++ b/5_Hardware/PCB_EXTENSION_CircuitVoyager_pre1/Project Outputs for PCB_EXT_CV_PRE1/BOM/BOM-PCB_EXT_CV_PRE1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe2074dc24c052ba/Beruflich/TBZ/Projects/CircuitVoyager_pre1/5_Hardware/PCB_EXTENSION_CircuitVoyager_pre1/Project Outputs for PCB_EXT_CV_PRE1/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{872B755E-4953-4036-87C6-0291E7E18A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41E92AA7-37DF-4921-9103-1EC3759D3DA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23625" yWindow="7125" windowWidth="23010" windowHeight="12105" xr2:uid="{1582C24C-77ED-4C13-8CA3-684AA7DF70E2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="16230" xr2:uid="{8B365ECE-2AC1-4DE3-BECA-39F345C05E5C}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-PCB_EXT_CV_PRE1" sheetId="1" r:id="rId1"/>
@@ -18,21 +18,10 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'BOM-PCB_EXT_CV_PRE1'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -74,7 +63,7 @@
     <t>Header 10x2 STMod+</t>
   </si>
   <si>
-    <t>Header 10x2, 2mm, RA, TH, Height 3.20mm/3.50mm,BF060-20A-B-0200-0280-0305-L-D</t>
+    <t>Header 10x2, 2mm, RA, TH, Height 3.20mm/3.50mm,BF060-20A-B-0400-0280-0305-L-D</t>
   </si>
   <si>
     <t>D1, D2</t>
@@ -270,7 +259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,7 +333,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -639,20 +628,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9F5A5A-704D-4634-9BB5-2F6DE85C774A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE10952F-1778-471F-8D64-D801E9C5E6F5}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="1" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -669,7 +658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -686,7 +675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -703,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -718,7 +707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -733,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -748,7 +737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -763,7 +752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -780,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -797,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -814,7 +803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -831,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -848,7 +837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -865,7 +854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -882,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -899,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -916,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
@@ -931,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>56</v>
       </c>
@@ -946,7 +935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -961,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -976,7 +965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>65</v>
       </c>
@@ -993,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>69</v>
       </c>
@@ -1010,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>72</v>
       </c>
@@ -1026,7 +1015,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>